<commit_message>
CV Codes for all models done
</commit_message>
<xml_diff>
--- a/model_result.xlsx
+++ b/model_result.xlsx
@@ -397,27 +397,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Freshness</t>
+          <t>Production_system</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>xgboost</t>
+          <t>svm</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.711358594235953</t>
+          <t>0.171147107609372</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.756102261883366</t>
+          <t>0.207770676738276</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>472</t>
+          <t>0 12 18 66 21 3 1 1 0 11 51 57 4 0 1 0 0 5 16 37 33 8 2 0 0 6 26 66 24 4 1 0 0 2 19 59 19 0 0 0 0 0 8 33 144 65 1 0 0 2 16 66 20 7 2 0 1 2 12 28 57 16 1 0</t>
         </is>
       </c>
     </row>
@@ -429,27 +429,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Production_system</t>
+          <t>Freshness</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>xgboost</t>
+          <t>svm</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.409384546271339</t>
+          <t>0.583380735800705</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.358267631065825</t>
+          <t>0.717757875888754</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>510 6 396 49</t>
         </is>
       </c>
     </row>
@@ -461,27 +461,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Freshness</t>
+          <t>Production_system</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>xgboost</t>
+          <t>svm</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.695354938271605</t>
+          <t>0.173928420014363</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.728600820357531</t>
+          <t>0.231955137665147</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>329</t>
+          <t>0 0 4 25 9 0 0 1 0 1 32 62 18 0 1 0 0 0 5 43 44 2 1 0 0 0 6 27 7 0 0 0 0 0 1 55 39 0 0 0 0 0 5 24 145 61 1 0 0 1 2 33 4 0 0 0 1 0 1 41 56 13 1 0</t>
         </is>
       </c>
     </row>
@@ -493,27 +493,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Production_system</t>
+          <t>Freshness</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>xgboost</t>
+          <t>svm</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.459475308641975</t>
+          <t>0.536465480987216</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.411323765352541</t>
+          <t>0.678776482745529</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>355 5 327 28</t>
         </is>
       </c>
     </row>
@@ -525,27 +525,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Freshness</t>
+          <t>Production_system</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>xgboost</t>
+          <t>svm</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.700132284341415</t>
+          <t>0.223592118035333</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.725739629597158</t>
+          <t>0.309105738378981</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>389</t>
+          <t>2 5 41 47 22 3 0 1 24 69 11 6 1 0 1 0 0 2 11 31 47 5 0 0 0 0 6 45 33 33 0 0 0 9 5 35 53 3 0 0 0 18 23 49 101 46 0 0 0 1 6 45 25 44 0 0 1 6 3 28 66 6 0 0</t>
         </is>
       </c>
     </row>
@@ -557,27 +557,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Production_system</t>
+          <t>Freshness</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>xgboost</t>
+          <t>svm</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.482756026496822</t>
+          <t>0.517770881278367</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.451951043205661</t>
+          <t>0.667311578386005</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>454 12 437 26</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
All model's cv result is out
</commit_message>
<xml_diff>
--- a/model_result.xlsx
+++ b/model_result.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,22 +402,22 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>svm</t>
+          <t>xgboost</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.171147107609372</t>
+          <t>0.41015274034142</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.207770676738276</t>
+          <t>0.364246344618564</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0 12 18 66 21 3 1 1 0 11 51 57 4 0 1 0 0 5 16 37 33 8 2 0 0 6 26 66 24 4 1 0 0 2 19 59 19 0 0 0 0 0 8 33 144 65 1 0 0 2 16 66 20 7 2 0 1 2 12 28 57 16 1 0</t>
+          <t>33 20 8 15 8 20 10 8 9 70 8 6 4 10 10 7 6 15 8 10 13 13 13 23 14 14 9 36 7 20 15 12 8 16 22 7 18 7 6 15 8 14 6 8 6 193 4 12 12 8 6 18 3 10 43 13 5 18 16 9 12 19 10 28</t>
         </is>
       </c>
     </row>
@@ -429,34 +429,34 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Freshness</t>
+          <t>Production_system</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>svm</t>
+          <t>random_forest</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.583380735800705</t>
+          <t>0.144379708341973</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.717757875888754</t>
+          <t>0.184145675188277</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>510 6 396 49</t>
+          <t>1 22 40 32 24 1 1 1 0 25 52 32 14 0 1 0 0 7 12 39 37 5 1 0 0 5 28 66 21 7 0 0 0 7 16 51 24 1 0 0 0 0 16 63 147 23 2 0 0 7 19 46 33 8 0 0 1 3 7 46 46 13 1 0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>TB</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -466,34 +466,34 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>svm</t>
+          <t>knn</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.173928420014363</t>
+          <t>0.326919621259244</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.231955137665147</t>
+          <t>0.28039315054854</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>0 0 4 25 9 0 0 1 0 1 32 62 18 0 1 0 0 0 5 43 44 2 1 0 0 0 6 27 7 0 0 0 0 0 1 55 39 0 0 0 0 0 5 24 145 61 1 0 0 1 2 33 4 0 0 0 1 0 1 41 56 13 1 0</t>
+          <t>25 29 3 16 11 24 7 7 13 59 9 11 16 5 2 9 9 19 12 14 10 16 7 14 17 18 12 25 11 22 16 6 8 22 12 11 14 15 6 11 10 22 9 12 9 162 7 20 13 12 14 18 6 7 26 17 4 20 10 11 16 26 11 19</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TB</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Freshness</t>
+          <t>Production_system</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -503,24 +503,24 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.536465480987216</t>
+          <t>0.180693033381713</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.678776482745529</t>
+          <t>0.223945571233309</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>355 5 327 28</t>
+          <t>0 11 18 68 20 2 2 1 0 15 47 57 4 0 1 0 0 3 19 35 37 6 1 0 0 8 20 71 25 2 1 0 0 1 21 58 19 0 0 0 0 0 8 31 151 61 0 0 0 3 16 68 17 5 4 0 1 2 11 29 56 18 0 0</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TP</t>
+          <t>OM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -530,54 +530,1014 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>svm</t>
+          <t>logistic_regression</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.223592118035333</t>
+          <t>0.677705611998065</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.309105738378981</t>
+          <t>0.636452603106343</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2 5 41 47 22 3 0 1 24 69 11 6 1 0 1 0 0 2 11 31 47 5 0 0 0 0 6 45 33 33 0 0 0 9 5 35 53 3 0 0 0 18 23 49 101 46 0 0 0 1 6 45 25 44 0 0 1 6 3 28 66 6 0 0</t>
+          <t>65 2 5 14 10 3 19 4 5 84 11 9 4 1 9 1 2 14 55 0 16 7 5 2 11 6 3 80 3 2 11 11 8 1 11 4 63 2 5 5 5 1 6 1 5 223 2 8 18 5 7 12 1 3 66 1 6 0 6 15 7 10 0 73</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>plsda</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>0.658585238308391</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0.62543679822207</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>69 8 0 17 8 0 14 6 10 89 3 12 2 0 7 1 5 11 50 7 12 7 2 7 16 8 2 75 4 1 12 9 0 4 12 6 62 2 5 8 2 1 17 8 4 206 1 12 20 8 2 18 2 0 61 2 4 0 11 4 3 17 1 77</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>xgboost</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>0.71898697214735</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>0.763392888949898</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>477 117 179 275</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>0.621684507780466</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>0.716783347550642</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>487 78 307 143</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>0.673161241274449</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>0.73467963779635</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>473 121 223 231</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>svm</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.581851003668739</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>0.716920212636243</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>509 6 397 49</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>logistic_regression</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.874784539360011</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0.888160306227683</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>529 65 68 386</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>OM</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>plsda</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.834730976570599</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0.856916633965787</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>517 77 98 356</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>xgboost</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>0.410183742528846</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>0.385570677648675</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>6 6 2 2 1 7 4 7 4 60 3 2 9 18 7 9 3 5 25 1 26 27 3 16 0 6 2 3 6 8 2 7 0 6 31 2 24 23 1 21 2 10 17 3 22 159 2 18 5 6 4 2 3 4 7 3 6 6 25 2 19 28 1 34</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>0.13039573684144</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>0.161952234777158</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>0 2 9 13 7 3 0 1 0 5 46 43 17 0 1 0 0 0 5 30 60 11 0 0 0 0 5 21 8 0 0 0 0 0 4 49 47 8 0 0 0 0 14 44 152 23 0 0 0 1 3 19 10 1 0 0 1 0 7 39 60 13 1 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>0.355163313257917</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>0.340369197462483</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>0 3 5 0 4 13 0 10 6 25 6 2 18 35 9 11 2 8 18 1 27 19 4 27 1 5 1 0 12 9 0 6 1 10 17 3 37 20 4 16 2 13 8 1 22 162 5 20 3 2 3 3 9 5 2 7 4 9 18 3 23 30 3 31</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>svm</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>0.162575820803669</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>0.243437000717556</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0 0 1 25 5 2 1 1 0 0 16 81 13 0 2 0 0 0 0 56 46 4 0 0 0 0 2 27 5 0 0 0 0 0 0 66 41 1 0 0 0 0 1 27 146 58 1 0 0 1 1 28 4 0 0 0 1 0 1 49 64 6 0 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>logistic_regression</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>0.777859920448195</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>0.749401882181997</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>21 4 1 3 1 0 4 1 4 81 8 0 6 4 3 6 1 1 71 3 8 11 1 10 0 0 0 27 1 1 5 0 2 0 7 1 86 4 0 8 0 2 12 1 3 200 1 14 3 1 1 2 0 0 24 3 3 0 5 1 5 13 1 93</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>plsda</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0.656563517539533</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>0.623477200518046</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>15 6 1 7 0 0 5 1 11 83 0 1 9 0 6 2 2 2 45 1 18 3 4 31 7 0 0 20 1 0 6 0 0 2 9 2 69 2 1 23 0 0 17 3 5 184 3 21 1 2 0 8 0 0 23 0 1 3 15 0 11 21 0 70</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>xgboost</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>0.706940777410464</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>0.739693582531339</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>329 97 132 219</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>0.658815235397514</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>0.736080734789246</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>367 52 211 137</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>0.646485992355413</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>0.698642380174603</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>318 108 168 183</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>svm</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>0.549995941183297</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>0.694056418569624</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>363 4 316 27</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>logistic_regression</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>0.927751279366869</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>0.934425705664881</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>394 32 26 325</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>TB</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>plsda</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>0.916091481248044</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>0.923944879685627</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>398 28 39 312</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>TP</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Freshness</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>xgboost</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>0.47725427799986</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>0.447489304360612</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>51 5 4 12 2 20 17 9 2 94 0 0 0 10 1 1 8 1 17 2 11 25 6 19 8 0 1 52 3 7 41 6 2 5 10 5 19 30 2 25 12 17 9 4 14 143 6 17 6 1 1 31 1 5 59 0 6 7 6 2 18 47 2 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>0.226928825653973</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>0.298646139336027</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>24 15 25 30 21 4 0 1 5 52 39 8 3 0 1 0 0 5 8 30 38 8 0 0 0 1 9 57 40 11 0 0 0 3 8 26 42 19 0 0 0 6 28 48 104 36 0 0 0 5 6 34 50 9 0 0 1 3 8 31 49 21 0 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>0.431475515463917</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>0.425641210742857</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>50 7 5 13 5 17 12 11 1 96 0 0 1 7 1 2 16 1 7 9 8 24 8 16 2 0 6 55 4 9 37 5 9 7 9 5 15 29 5 19 19 27 9 6 12 115 8 26 4 1 1 34 1 3 60 0 11 8 16 3 13 42 2 18</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
         <is>
           <t>svm</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>0.517770881278367</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>0.667311578386005</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>454 12 437 26</t>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>0.237409706150501</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>0.32551200686731</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>1 7 44 43 23 1 0 1 17 72 13 4 1 0 1 0 0 1 9 27 48 4 0 0 0 0 10 58 49 1 0 0 0 7 4 29 55 3 0 0 0 20 21 46 101 34 0 0 0 1 22 35 46 0 0 0 1 6 4 27 69 6 0 0</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>logistic_regression</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>0.691875964303247</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>0.669397621793202</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>87 3 4 6 2 4 12 2 5 71 4 3 6 3 9 7 2 1 51 1 17 11 0 6 6 0 4 84 4 2 12 6 3 0 15 2 64 6 1 7 2 1 9 4 9 174 0 23 12 4 4 8 2 3 69 2 3 2 7 3 4 24 3 67</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Production_system</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>plsda</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>0.65981529209622</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>0.63329725393548</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>79 8 0 10 0 2 20 1 6 95 0 4 1 0 1 1 5 1 27 4 26 14 2 10 12 0 1 82 1 1 19 2 1 0 18 1 54 2 0 22 5 0 13 7 3 163 2 29 15 1 2 22 0 1 63 0 2 0 5 0 9 24 0 73</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>xgboost</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>0.688770907847675</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>0.704807922153466</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>365 156 146 299</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>random_forest</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>0.646136913095331</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>0.715053297298479</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>415 66 261 178</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>knn</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>0.688756443298969</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>0.706753273040363</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>365 156 146 299</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>svm</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>0.510394236925982</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>0.667381975090866</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>431 11 421 15</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>logistic_regression</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>0.88702442317133</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>0.893271999775081</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>465 56 55 390</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Freshness</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>plsda</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>0.873528780068728</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>0.879450218603107</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>451 70 54 391</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Preprocessing order is now corrected
</commit_message>
<xml_diff>
--- a/model_result.xlsx
+++ b/model_result.xlsx
@@ -407,17 +407,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.41015274034142</t>
+          <t>0.395815018315018</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.364246344618564</t>
+          <t>0.348539223534064</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>33 20 8 15 8 20 10 8 9 70 8 6 4 10 10 7 6 15 8 10 13 13 13 23 14 14 9 36 7 20 15 12 8 16 22 7 18 7 6 15 8 14 6 8 6 193 4 12 12 8 6 18 3 10 43 13 5 18 16 9 12 19 10 28</t>
+          <t>35 22 2 20 9 20 12 2 13 66 6 8 5 11 8 7 4 16 10 10 14 12 15 19 15 12 6 37 7 15 17 18 9 13 16 11 17 6 4 20 8 12 6 3 10 188 5 18 16 7 4 23 4 10 39 10 5 18 12 15 12 24 11 20</t>
         </is>
       </c>
     </row>
@@ -439,17 +439,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.144379708341973</t>
+          <t>0.133571428571429</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>0.184145675188277</t>
+          <t>0.177444139784643</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>1 22 40 32 24 1 1 1 0 25 52 32 14 0 1 0 0 7 12 39 37 5 1 0 0 5 28 66 21 7 0 0 0 7 16 51 24 1 0 0 0 0 16 63 147 23 2 0 0 7 19 46 33 8 0 0 1 3 7 46 46 13 1 0</t>
+          <t>1 16 43 35 23 3 0 1 0 28 47 35 12 1 1 0 0 8 14 40 32 5 1 0 0 5 31 53 31 7 0 0 0 6 15 49 20 6 0 0 0 0 14 66 146 23 1 0 0 6 17 46 35 9 0 0 1 3 8 43 50 12 0 0</t>
         </is>
       </c>
     </row>
@@ -471,17 +471,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.326919621259244</t>
+          <t>0.348727106227106</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>0.28039315054854</t>
+          <t>0.302780440985067</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>25 29 3 16 11 24 7 7 13 59 9 11 16 5 2 9 9 19 12 14 10 16 7 14 17 18 12 25 11 22 16 6 8 22 12 11 14 15 6 11 10 22 9 12 9 162 7 20 13 12 14 18 6 7 26 17 4 20 10 11 16 26 11 19</t>
+          <t>32 22 6 20 8 22 6 6 13 65 6 8 12 4 5 11 8 17 13 22 8 11 10 11 16 12 12 31 10 23 14 9 10 23 10 10 16 9 5 13 12 20 6 13 11 160 11 17 12 13 14 22 9 8 25 10 5 19 7 12 16 27 10 21</t>
         </is>
       </c>
     </row>
@@ -503,17 +503,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.180693033381713</t>
+          <t>0.184441391941392</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>0.223945571233309</t>
+          <t>0.238148451413268</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>0 11 18 68 20 2 2 1 0 15 47 57 4 0 1 0 0 3 19 35 37 6 1 0 0 8 20 71 25 2 1 0 0 1 21 58 19 0 0 0 0 0 8 31 151 61 0 0 0 3 16 68 17 5 4 0 1 2 11 29 56 18 0 0</t>
+          <t>2 14 19 63 19 2 2 1 0 23 44 54 2 0 1 0 0 5 15 36 34 9 1 0 0 10 24 64 26 2 1 0 0 3 17 55 19 2 0 0 0 1 10 31 140 66 2 0 0 4 21 57 22 6 3 0 1 4 10 33 50 19 0 0</t>
         </is>
       </c>
     </row>
@@ -535,17 +535,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.677705611998065</t>
+          <t>0.716584249084249</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>0.636452603106343</t>
+          <t>0.676290032580206</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>65 2 5 14 10 3 19 4 5 84 11 9 4 1 9 1 2 14 55 0 16 7 5 2 11 6 3 80 3 2 11 11 8 1 11 4 63 2 5 5 5 1 6 1 5 223 2 8 18 5 7 12 1 3 66 1 6 0 6 15 7 10 0 73</t>
+          <t>67 8 5 15 12 1 12 2 2 95 11 5 1 1 7 2 2 15 55 1 10 7 4 6 5 2 4 88 3 2 10 13 8 1 9 3 65 2 6 2 4 3 7 0 4 218 2 12 14 8 6 9 1 1 71 3 5 0 2 12 4 6 1 87</t>
         </is>
       </c>
     </row>
@@ -567,17 +567,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>0.658585238308391</t>
+          <t>0.649395604395604</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>0.62543679822207</t>
+          <t>0.612337723815009</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>69 8 0 17 8 0 14 6 10 89 3 12 2 0 7 1 5 11 50 7 12 7 2 7 16 8 2 75 4 1 12 9 0 4 12 6 62 2 5 8 2 1 17 8 4 206 1 12 20 8 2 18 2 0 61 2 4 0 11 4 3 17 1 77</t>
+          <t>65 11 0 18 6 0 15 7 10 86 2 16 3 0 6 1 2 12 49 7 11 7 3 9 17 11 3 72 4 1 11 8 0 8 9 5 60 0 4 10 2 1 12 9 2 211 0 13 17 12 3 20 1 0 57 3 4 1 13 4 4 13 2 76</t>
         </is>
       </c>
     </row>
@@ -599,17 +599,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>0.71898697214735</t>
+          <t>0.708946886446887</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>0.763392888949898</t>
+          <t>0.74888662732155</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>477 117 179 275</t>
+          <t>457 134 171 281</t>
         </is>
       </c>
     </row>
@@ -631,17 +631,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>0.621684507780466</t>
+          <t>0.630602564102564</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>0.716783347550642</t>
+          <t>0.726205632697215</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>487 78 307 143</t>
+          <t>509 75 307 141</t>
         </is>
       </c>
     </row>
@@ -663,17 +663,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>0.673161241274449</t>
+          <t>0.665732600732601</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>0.73467963779635</t>
+          <t>0.7223646814042</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>473 121 223 231</t>
+          <t>458 133 217 235</t>
         </is>
       </c>
     </row>
@@ -695,17 +695,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>0.581851003668739</t>
+          <t>0.584171049438056</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>0.716920212636243</t>
+          <t>0.718593786714015</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>509 6 397 49</t>
+          <t>514 9 393 49</t>
         </is>
       </c>
     </row>
@@ -727,17 +727,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>0.874784539360011</t>
+          <t>0.880842490842491</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>0.888160306227683</t>
+          <t>0.893022489407028</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>529 65 68 386</t>
+          <t>528 63 63 389</t>
         </is>
       </c>
     </row>
@@ -759,17 +759,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>0.834730976570599</t>
+          <t>0.839606227106227</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>0.856916633965787</t>
+          <t>0.858771206470602</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>517 77 98 356</t>
+          <t>514 77 92 360</t>
         </is>
       </c>
     </row>
@@ -791,17 +791,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.410183742528846</t>
+          <t>0.430193490719806</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>0.385570677648675</t>
+          <t>0.402392095966843</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>6 6 2 2 1 7 4 7 4 60 3 2 9 18 7 9 3 5 25 1 26 27 3 16 0 6 2 3 6 8 2 7 0 6 31 2 24 23 1 21 2 10 17 3 22 159 2 18 5 6 4 2 3 4 7 3 6 6 25 2 19 28 1 34</t>
+          <t>7 9 3 1 1 12 3 6 5 67 6 5 4 10 6 9 2 2 21 3 20 20 3 25 3 8 3 6 3 5 2 4 2 3 18 3 33 14 6 25 9 11 21 3 12 148 1 18 5 5 5 3 0 6 9 6 4 8 22 1 23 23 6 40</t>
         </is>
       </c>
     </row>
@@ -823,17 +823,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>0.13039573684144</t>
+          <t>0.137825332562175</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>0.161952234777158</t>
+          <t>0.184425612287826</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>0 2 9 13 7 3 0 1 0 5 46 43 17 0 1 0 0 0 5 30 60 11 0 0 0 0 5 21 8 0 0 0 0 0 4 49 47 8 0 0 0 0 14 44 152 23 0 0 0 1 3 19 10 1 0 0 1 0 7 39 60 13 1 0</t>
+          <t>0 4 10 15 10 2 0 1 0 8 48 41 13 1 1 0 0 0 4 31 50 11 0 0 0 2 7 20 5 0 0 0 0 0 4 42 48 10 0 0 0 0 15 53 129 26 0 0 0 1 0 20 17 1 0 0 1 0 8 34 59 23 2 0</t>
         </is>
       </c>
     </row>
@@ -855,17 +855,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>0.355163313257917</t>
+          <t>0.343455228981545</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>0.340369197462483</t>
+          <t>0.315048126524228</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>0 3 5 0 4 13 0 10 6 25 6 2 18 35 9 11 2 8 18 1 27 19 4 27 1 5 1 0 12 9 0 6 1 10 17 3 37 20 4 16 2 13 8 1 22 162 5 20 3 2 3 3 9 5 2 7 4 9 18 3 23 30 3 31</t>
+          <t>5 3 2 1 3 15 4 9 4 28 7 4 15 30 8 16 2 7 14 1 21 15 5 31 1 4 4 4 9 6 0 6 3 10 10 5 28 21 9 18 4 11 15 2 16 154 4 17 5 6 3 1 8 11 0 5 6 17 22 2 18 28 3 31</t>
         </is>
       </c>
     </row>
@@ -887,17 +887,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>0.162575820803669</t>
+          <t>0.156261959226649</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>0.243437000717556</t>
+          <t>0.21978729702227</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0 0 1 25 5 2 1 1 0 0 16 81 13 0 2 0 0 0 0 56 46 4 0 0 0 0 2 27 5 0 0 0 0 0 0 66 41 1 0 0 0 0 1 27 146 58 1 0 0 1 1 28 4 0 0 0 1 0 1 49 64 6 0 0</t>
+          <t>0 0 8 21 10 2 0 1 0 1 23 68 19 0 1 0 0 0 2 45 45 4 0 0 0 0 5 24 5 0 0 0 0 0 1 57 44 2 0 0 0 0 5 26 141 49 2 0 0 1 4 26 7 1 0 0 1 0 2 51 61 9 3 0</t>
         </is>
       </c>
     </row>
@@ -919,17 +919,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0.777859920448195</t>
+          <t>0.791954216669406</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>0.749401882181997</t>
+          <t>0.772167202712456</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>21 4 1 3 1 0 4 1 4 81 8 0 6 4 3 6 1 1 71 3 8 11 1 10 0 0 0 27 1 1 5 0 2 0 7 1 86 4 0 8 0 2 12 1 3 200 1 14 3 1 1 2 0 0 24 3 3 0 5 1 5 13 1 93</t>
+          <t>30 2 1 3 1 0 2 3 6 85 5 0 7 3 1 5 3 2 69 0 11 8 0 3 5 0 0 25 1 0 2 1 2 0 6 2 82 2 0 10 3 1 7 2 7 188 1 14 2 1 0 1 0 1 33 1 2 1 8 0 6 13 0 97</t>
         </is>
       </c>
     </row>
@@ -951,17 +951,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>0.656563517539533</t>
+          <t>0.672211122211122</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>0.623477200518046</t>
+          <t>0.640772313691266</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>15 6 1 7 0 0 5 1 11 83 0 1 9 0 6 2 2 2 45 1 18 3 4 31 7 0 0 20 1 0 6 0 0 2 9 2 69 2 1 23 0 0 17 3 5 184 3 21 1 2 0 8 0 0 23 0 1 3 15 0 11 21 0 70</t>
+          <t>24 4 0 5 0 0 8 1 12 87 0 2 4 0 5 2 1 1 35 0 20 5 7 27 8 0 0 22 1 0 3 0 0 0 12 1 68 2 1 20 0 0 10 1 4 176 6 26 4 3 0 7 0 0 25 0 1 4 14 1 13 14 0 80</t>
         </is>
       </c>
     </row>
@@ -983,17 +983,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>0.706940777410464</t>
+          <t>0.69037015615963</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>0.739693582531339</t>
+          <t>0.730581642751703</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>329 97 132 219</t>
+          <t>325 94 146 206</t>
         </is>
       </c>
     </row>
@@ -1015,17 +1015,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>0.658815235397514</t>
+          <t>0.624942277926798</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>0.736080734789246</t>
+          <t>0.706727604309903</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>367 52 211 137</t>
+          <t>348 57 227 122</t>
         </is>
       </c>
     </row>
@@ -1047,17 +1047,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>0.646485992355413</t>
+          <t>0.65144986592355</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>0.698642380174603</t>
+          <t>0.692168112150492</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>318 108 168 183</t>
+          <t>307 112 158 194</t>
         </is>
       </c>
     </row>
@@ -1079,17 +1079,17 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>0.549995941183297</t>
+          <t>0.546113973101113</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>0.694056418569624</t>
+          <t>0.68934280694311</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>363 4 316 27</t>
+          <t>356 4 317 27</t>
         </is>
       </c>
     </row>
@@ -1111,17 +1111,17 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>0.927751279366869</t>
+          <t>0.901085806265686</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>0.934425705664881</t>
+          <t>0.907443140544242</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>394 32 26 325</t>
+          <t>375 44 34 318</t>
         </is>
       </c>
     </row>
@@ -1143,17 +1143,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>0.916091481248044</t>
+          <t>0.916743344374923</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>0.923944879685627</t>
+          <t>0.922716645570181</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>398 28 39 312</t>
+          <t>386 33 33 319</t>
         </is>
       </c>
     </row>
@@ -1175,17 +1175,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>0.47725427799986</t>
+          <t>0.475040404040404</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>0.447489304360612</t>
+          <t>0.456021509456203</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>51 5 4 12 2 20 17 9 2 94 0 0 0 10 1 1 8 1 17 2 11 25 6 19 8 0 1 52 3 7 41 6 2 5 10 5 19 30 2 25 12 17 9 4 14 143 6 17 6 1 1 31 1 5 59 0 6 7 6 2 18 47 2 25</t>
+          <t>48 4 7 13 4 16 11 6 0 108 0 0 0 12 1 1 9 0 12 2 12 38 8 14 9 0 2 48 4 9 41 2 3 8 16 5 15 32 0 17 15 19 9 4 15 161 4 22 5 1 0 37 1 2 59 0 10 4 12 4 12 50 0 23</t>
         </is>
       </c>
     </row>
@@ -1207,17 +1207,17 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>0.226928825653973</t>
+          <t>0.219333333333333</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>0.298646139336027</t>
+          <t>0.287490100112788</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>24 15 25 30 21 4 0 1 5 52 39 8 3 0 1 0 0 5 8 30 38 8 0 0 0 1 9 57 40 11 0 0 0 3 8 26 42 19 0 0 0 6 28 48 104 36 0 0 0 5 6 34 50 9 0 0 1 3 8 31 49 21 0 0</t>
+          <t>7 18 24 32 22 5 0 1 2 78 33 6 2 0 1 0 0 4 13 31 36 11 0 0 0 4 12 39 49 11 0 0 0 3 12 29 43 8 1 0 1 6 25 54 124 39 0 0 1 2 9 31 54 8 0 0 2 0 11 25 59 16 2 0</t>
         </is>
       </c>
     </row>
@@ -1239,17 +1239,17 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>0.431475515463917</t>
+          <t>0.411979797979798</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>0.425641210742857</t>
+          <t>0.40842324409854</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>50 7 5 13 5 17 12 11 1 96 0 0 1 7 1 2 16 1 7 9 8 24 8 16 2 0 6 55 4 9 37 5 9 7 9 5 15 29 5 19 19 27 9 6 12 115 8 26 4 1 1 34 1 3 60 0 11 8 16 3 13 42 2 18</t>
+          <t>34 3 6 9 11 18 17 11 0 108 0 0 2 11 1 0 10 1 11 12 10 23 9 19 8 0 5 42 4 9 43 4 7 10 11 9 7 30 7 15 21 24 17 6 16 120 11 34 3 1 1 38 1 3 58 0 8 5 10 3 11 47 0 31</t>
         </is>
       </c>
     </row>
@@ -1271,17 +1271,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>0.237409706150501</t>
+          <t>0.251484848484848</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>0.32551200686731</t>
+          <t>0.333692644826796</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1 7 44 43 23 1 0 1 17 72 13 4 1 0 1 0 0 1 9 27 48 4 0 0 0 0 10 58 49 1 0 0 0 7 4 29 55 3 0 0 0 20 21 46 101 34 0 0 0 1 22 35 46 0 0 0 1 6 4 27 69 6 0 0</t>
+          <t>0 3 34 44 22 5 0 1 22 81 12 5 0 1 1 0 0 2 11 26 53 3 0 0 0 0 12 51 40 12 0 0 0 9 2 30 49 6 0 0 0 18 16 45 111 59 0 0 0 1 14 35 46 9 0 0 2 4 1 22 70 16 0 0</t>
         </is>
       </c>
     </row>
@@ -1303,17 +1303,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>0.691875964303247</t>
+          <t>0.739571428571429</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>0.669397621793202</t>
+          <t>0.711403975928663</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>87 3 4 6 2 4 12 2 5 71 4 3 6 3 9 7 2 1 51 1 17 11 0 6 6 0 4 84 4 2 12 6 3 0 15 2 64 6 1 7 2 1 9 4 9 174 0 23 12 4 4 8 2 3 69 2 3 2 7 3 4 24 3 67</t>
+          <t>77 3 1 8 2 2 12 4 5 93 3 2 6 4 4 5 2 2 59 2 13 9 1 7 11 0 1 80 2 3 13 5 1 0 16 1 68 3 3 4 0 3 8 1 6 210 2 19 9 3 6 9 1 3 71 3 3 1 5 1 6 18 1 80</t>
         </is>
       </c>
     </row>
@@ -1335,17 +1335,17 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>0.65981529209622</t>
+          <t>0.686434343434344</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>0.63329725393548</t>
+          <t>0.644617567573662</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>79 8 0 10 0 2 20 1 6 95 0 4 1 0 1 1 5 1 27 4 26 14 2 10 12 0 1 82 1 1 19 2 1 0 18 1 54 2 0 22 5 0 13 7 3 163 2 29 15 1 2 22 0 1 63 0 2 0 5 0 9 24 0 73</t>
+          <t>74 5 0 14 0 2 11 3 4 116 0 1 0 0 1 0 7 0 31 7 23 11 3 13 13 0 1 79 1 1 18 2 2 1 14 3 56 0 0 20 4 1 10 3 4 201 7 19 10 1 3 32 0 1 58 0 2 3 6 0 5 29 0 70</t>
         </is>
       </c>
     </row>
@@ -1367,17 +1367,17 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>0.688770907847675</t>
+          <t>0.688313131313131</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>0.704807922153466</t>
+          <t>0.706664179894771</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>365 156 146 299</t>
+          <t>374 168 145 313</t>
         </is>
       </c>
     </row>
@@ -1399,17 +1399,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>0.646136913095331</t>
+          <t>0.603138818129754</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>0.715053297298479</t>
+          <t>0.690561384065252</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>415 66 261 178</t>
+          <t>433 90 297 154</t>
         </is>
       </c>
     </row>
@@ -1431,17 +1431,17 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>0.688756443298969</t>
+          <t>0.693414141414141</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>0.706753273040363</t>
+          <t>0.710760179334855</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>365 156 146 299</t>
+          <t>383 159 149 309</t>
         </is>
       </c>
     </row>
@@ -1463,17 +1463,17 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>0.510394236925982</t>
+          <t>0.52787357837508</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>0.667381975090866</t>
+          <t>0.676525538451507</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>431 11 421 15</t>
+          <t>451 13 419 27</t>
         </is>
       </c>
     </row>
@@ -1495,17 +1495,17 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>0.88702442317133</t>
+          <t>0.903787878787879</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>0.893271999775081</t>
+          <t>0.908763589355317</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>465 56 55 390</t>
+          <t>491 51 47 411</t>
         </is>
       </c>
     </row>
@@ -1527,17 +1527,17 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>0.873528780068728</t>
+          <t>0.870727272727273</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>0.879450218603107</t>
+          <t>0.876582256910554</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>451 70 54 391</t>
+          <t>467 75 56 402</t>
         </is>
       </c>
     </row>

</xml_diff>